<commit_message>
Renamed "Shrub" to "CSS"
Ashish originally called what I call as "CSS", as "Shrub", so I simply renamed this vegetation treatment back to "CSS" to match with my enzyme activity data and to facilitate the use of my existing code
</commit_message>
<xml_diff>
--- a/Statistical analyses/Tukey posthoc/C_O_stretching/C_O_stretching, Vegetation, groups, annotated.xlsx
+++ b/Statistical analyses/Tukey posthoc/C_O_stretching/C_O_stretching, Vegetation, groups, annotated.xlsx
@@ -22,10 +22,10 @@
     <t>labels</t>
   </si>
   <si>
+    <t>CSS</t>
+  </si>
+  <si>
     <t>Grassland</t>
-  </si>
-  <si>
-    <t>Shrub</t>
   </si>
   <si>
     <t>a</t>

</xml_diff>